<commit_message>
add some files, updates, store now all results in the same Databank
</commit_message>
<xml_diff>
--- a/engine/data/additional_engines.xlsx
+++ b/engine/data/additional_engines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB6B57F-4363-486F-B862-AFBB749DCC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23B7EC3-FCE5-4FA0-A844-1639D2FF96D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>

</xml_diff>